<commit_message>
Tabellen als afbeelding voor gDocs
</commit_message>
<xml_diff>
--- a/ass_3/Table and Chart of communities per year/Yearly Growth and Shrinkage per community.xlsx
+++ b/ass_3/Table and Chart of communities per year/Yearly Growth and Shrinkage per community.xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guido/Development/WebAnalyticsHadoop/GitHub/web-analytics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guido/Development/WebAnalyticsHadoop/GitHub/web-analytics/ass_3/Table and Chart of communities per year/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,9 +50,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Number of publications</t>
-  </si>
-  <si>
     <t>Relative share of attention</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>2010</t>
+  </si>
+  <si>
+    <t>Number of authors</t>
   </si>
 </sst>
 </file>
@@ -170,41 +170,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -437,7 +402,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -455,6 +419,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -661,6 +626,41 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -706,7 +706,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Absolute number of publications per comm.</a:t>
+              <a:t>Absolute number of authors per comm.</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1386,11 +1386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2095462032"/>
-        <c:axId val="-2088948752"/>
+        <c:axId val="-2114548208"/>
+        <c:axId val="-2118014640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095462032"/>
+        <c:axId val="-2114548208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1433,7 +1433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088948752"/>
+        <c:crossAx val="-2118014640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1441,7 +1441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088948752"/>
+        <c:axId val="-2118014640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1492,7 +1492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095462032"/>
+        <c:crossAx val="-2114548208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2288,11 +2288,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2137864800"/>
-        <c:axId val="-2080561648"/>
+        <c:axId val="2131817728"/>
+        <c:axId val="2131825376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137864800"/>
+        <c:axId val="2131817728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2335,7 +2335,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080561648"/>
+        <c:crossAx val="2131825376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2343,7 +2343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080561648"/>
+        <c:axId val="2131825376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2394,7 +2394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137864800"/>
+        <c:crossAx val="2131817728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3653,62 +3653,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:L11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:L11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A4:L11"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Number of publications" dataDxfId="27"/>
-    <tableColumn id="2" name="2001" dataDxfId="26"/>
-    <tableColumn id="3" name="2002" dataDxfId="25"/>
-    <tableColumn id="4" name="2003" dataDxfId="24"/>
-    <tableColumn id="5" name="2004" dataDxfId="23"/>
-    <tableColumn id="6" name="2005" dataDxfId="22"/>
-    <tableColumn id="7" name="2006" dataDxfId="21"/>
-    <tableColumn id="8" name="2007" dataDxfId="20"/>
-    <tableColumn id="9" name="2008" dataDxfId="19"/>
-    <tableColumn id="10" name="2009" dataDxfId="18"/>
-    <tableColumn id="11" name="2010" dataDxfId="17"/>
-    <tableColumn id="12" name="Total" dataDxfId="16"/>
+    <tableColumn id="1" name="Number of authors" dataDxfId="25"/>
+    <tableColumn id="2" name="2001" dataDxfId="24"/>
+    <tableColumn id="3" name="2002" dataDxfId="23"/>
+    <tableColumn id="4" name="2003" dataDxfId="22"/>
+    <tableColumn id="5" name="2004" dataDxfId="21"/>
+    <tableColumn id="6" name="2005" dataDxfId="20"/>
+    <tableColumn id="7" name="2006" dataDxfId="19"/>
+    <tableColumn id="8" name="2007" dataDxfId="18"/>
+    <tableColumn id="9" name="2008" dataDxfId="17"/>
+    <tableColumn id="10" name="2009" dataDxfId="16"/>
+    <tableColumn id="11" name="2010" dataDxfId="15"/>
+    <tableColumn id="12" name="Total" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A14:L20" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A14:L20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A14:L20"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Relative share of attention" dataDxfId="13"/>
-    <tableColumn id="2" name="2001" dataDxfId="12">
+    <tableColumn id="1" name="Relative share of attention" dataDxfId="11"/>
+    <tableColumn id="2" name="2001" dataDxfId="10">
       <calculatedColumnFormula>B5/B$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2002" dataDxfId="11">
+    <tableColumn id="3" name="2002" dataDxfId="9">
       <calculatedColumnFormula>C5/C$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="2003" dataDxfId="10">
+    <tableColumn id="4" name="2003" dataDxfId="8">
       <calculatedColumnFormula>D5/D$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="2004" dataDxfId="9">
+    <tableColumn id="5" name="2004" dataDxfId="7">
       <calculatedColumnFormula>E5/E$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="2005" dataDxfId="8">
+    <tableColumn id="6" name="2005" dataDxfId="6">
       <calculatedColumnFormula>F5/F$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="2006" dataDxfId="7">
+    <tableColumn id="7" name="2006" dataDxfId="5">
       <calculatedColumnFormula>G5/G$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="2007" dataDxfId="6">
+    <tableColumn id="8" name="2007" dataDxfId="4">
       <calculatedColumnFormula>H5/H$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="2008" dataDxfId="5">
+    <tableColumn id="9" name="2008" dataDxfId="3">
       <calculatedColumnFormula>I5/I$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="2009" dataDxfId="4">
+    <tableColumn id="10" name="2009" dataDxfId="2">
       <calculatedColumnFormula>J5/J$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="2010" dataDxfId="3">
+    <tableColumn id="11" name="2010" dataDxfId="1">
       <calculatedColumnFormula>K5/K$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Total" dataDxfId="2">
+    <tableColumn id="12" name="Total" dataDxfId="0">
       <calculatedColumnFormula>L5/L$11</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3979,10 +3979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M24"/>
+  <dimension ref="A2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3999,37 +3999,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>7</v>
@@ -4070,7 +4070,7 @@
         <v>720</v>
       </c>
       <c r="L5" s="1">
-        <f>SUM(B5:K5)</f>
+        <f t="shared" ref="L5:L10" si="0">SUM(B5:K5)</f>
         <v>7666</v>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
         <v>1330</v>
       </c>
       <c r="L6" s="1">
-        <f>SUM(B6:K6)</f>
+        <f t="shared" si="0"/>
         <v>11601</v>
       </c>
     </row>
@@ -4148,7 +4148,7 @@
         <v>603</v>
       </c>
       <c r="L7" s="1">
-        <f>SUM(B7:K7)</f>
+        <f t="shared" si="0"/>
         <v>4374</v>
       </c>
     </row>
@@ -4187,7 +4187,7 @@
         <v>1058</v>
       </c>
       <c r="L8" s="1">
-        <f>SUM(B8:K8)</f>
+        <f t="shared" si="0"/>
         <v>9100</v>
       </c>
     </row>
@@ -4226,7 +4226,7 @@
         <v>627</v>
       </c>
       <c r="L9" s="1">
-        <f>SUM(B9:K9)</f>
+        <f t="shared" si="0"/>
         <v>5817</v>
       </c>
     </row>
@@ -4265,7 +4265,7 @@
         <v>1419</v>
       </c>
       <c r="L10" s="1">
-        <f>SUM(B10:K10)</f>
+        <f t="shared" si="0"/>
         <v>9301</v>
       </c>
     </row>
@@ -4274,83 +4274,83 @@
         <v>7</v>
       </c>
       <c r="B11" s="1">
-        <f>SUM(B5:B10)</f>
+        <f t="shared" ref="B11:L11" si="1">SUM(B5:B10)</f>
         <v>3074</v>
       </c>
       <c r="C11" s="1">
-        <f>SUM(C5:C10)</f>
+        <f t="shared" si="1"/>
         <v>2557</v>
       </c>
       <c r="D11" s="1">
-        <f>SUM(D5:D10)</f>
+        <f t="shared" si="1"/>
         <v>3836</v>
       </c>
       <c r="E11" s="1">
-        <f>SUM(E5:E10)</f>
+        <f t="shared" si="1"/>
         <v>3464</v>
       </c>
       <c r="F11" s="1">
-        <f>SUM(F5:F10)</f>
+        <f t="shared" si="1"/>
         <v>5198</v>
       </c>
       <c r="G11" s="1">
-        <f>SUM(G5:G10)</f>
+        <f t="shared" si="1"/>
         <v>4494</v>
       </c>
       <c r="H11" s="1">
-        <f>SUM(H5:H10)</f>
+        <f t="shared" si="1"/>
         <v>7294</v>
       </c>
       <c r="I11" s="1">
-        <f>SUM(I5:I10)</f>
+        <f t="shared" si="1"/>
         <v>5780</v>
       </c>
       <c r="J11" s="1">
-        <f>SUM(J5:J10)</f>
+        <f t="shared" si="1"/>
         <v>6405</v>
       </c>
       <c r="K11" s="1">
-        <f>SUM(K5:K10)</f>
+        <f t="shared" si="1"/>
         <v>5757</v>
       </c>
       <c r="L11" s="1">
-        <f>SUM(L5:L10)</f>
+        <f t="shared" si="1"/>
         <v>47859</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>7</v>
@@ -4361,47 +4361,47 @@
         <v>1</v>
       </c>
       <c r="B15" s="6">
-        <f>B5/B$11</f>
+        <f t="shared" ref="B15:L15" si="2">B5/B$11</f>
         <v>0.17989590110605075</v>
       </c>
       <c r="C15" s="6">
-        <f>C5/C$11</f>
+        <f t="shared" si="2"/>
         <v>0.24990222917481422</v>
       </c>
       <c r="D15" s="6">
-        <f>D5/D$11</f>
+        <f t="shared" si="2"/>
         <v>0.16032325338894682</v>
       </c>
       <c r="E15" s="6">
-        <f>E5/E$11</f>
+        <f t="shared" si="2"/>
         <v>0.22950346420323325</v>
       </c>
       <c r="F15" s="6">
-        <f>F5/F$11</f>
+        <f t="shared" si="2"/>
         <v>0.15294343978453251</v>
       </c>
       <c r="G15" s="6">
-        <f>G5/G$11</f>
+        <f t="shared" si="2"/>
         <v>0.21117044948820649</v>
       </c>
       <c r="H15" s="6">
-        <f>H5/H$11</f>
+        <f t="shared" si="2"/>
         <v>0.12462297778996435</v>
       </c>
       <c r="I15" s="6">
-        <f>I5/I$11</f>
+        <f t="shared" si="2"/>
         <v>0.13961937716262976</v>
       </c>
       <c r="J15" s="6">
-        <f>J5/J$11</f>
+        <f t="shared" si="2"/>
         <v>0.13801717408274786</v>
       </c>
       <c r="K15" s="6">
-        <f>K5/K$11</f>
+        <f t="shared" si="2"/>
         <v>0.12506513809275666</v>
       </c>
       <c r="L15" s="2">
-        <f>L5/L$11</f>
+        <f t="shared" si="2"/>
         <v>0.16017885873085522</v>
       </c>
     </row>
@@ -4410,47 +4410,47 @@
         <v>2</v>
       </c>
       <c r="B16" s="6">
-        <f>B6/B$11</f>
+        <f t="shared" ref="B16:L16" si="3">B6/B$11</f>
         <v>0.23259596616785946</v>
       </c>
       <c r="C16" s="6">
-        <f>C6/C$11</f>
+        <f t="shared" si="3"/>
         <v>0.11224090731325773</v>
       </c>
       <c r="D16" s="6">
-        <f>D6/D$11</f>
+        <f t="shared" si="3"/>
         <v>0.24739311783107404</v>
       </c>
       <c r="E16" s="6">
-        <f>E6/E$11</f>
+        <f t="shared" si="3"/>
         <v>0.22921478060046188</v>
       </c>
       <c r="F16" s="6">
-        <f>F6/F$11</f>
+        <f t="shared" si="3"/>
         <v>0.34724894190073102</v>
       </c>
       <c r="G16" s="6">
-        <f>G6/G$11</f>
+        <f t="shared" si="3"/>
         <v>0.27214063195371607</v>
       </c>
       <c r="H16" s="6">
-        <f>H6/H$11</f>
+        <f t="shared" si="3"/>
         <v>0.28831916643816835</v>
       </c>
       <c r="I16" s="6">
-        <f>I6/I$11</f>
+        <f t="shared" si="3"/>
         <v>0.20449826989619377</v>
       </c>
       <c r="J16" s="6">
-        <f>J6/J$11</f>
+        <f t="shared" si="3"/>
         <v>0.18938329430132708</v>
       </c>
       <c r="K16" s="6">
-        <f>K6/K$11</f>
+        <f t="shared" si="3"/>
         <v>0.23102310231023102</v>
       </c>
       <c r="L16" s="2">
-        <f>L6/L$11</f>
+        <f t="shared" si="3"/>
         <v>0.24239954867423055</v>
       </c>
     </row>
@@ -4459,47 +4459,47 @@
         <v>3</v>
       </c>
       <c r="B17" s="6">
-        <f>B7/B$11</f>
+        <f t="shared" ref="B17:L17" si="4">B7/B$11</f>
         <v>6.2459336369551074E-2</v>
       </c>
       <c r="C17" s="6">
-        <f>C7/C$11</f>
+        <f t="shared" si="4"/>
         <v>0.10833007430582714</v>
       </c>
       <c r="D17" s="6">
-        <f>D7/D$11</f>
+        <f t="shared" si="4"/>
         <v>9.5672575599582893E-2</v>
       </c>
       <c r="E17" s="6">
-        <f>E7/E$11</f>
+        <f t="shared" si="4"/>
         <v>9.6709006928406463E-2</v>
       </c>
       <c r="F17" s="6">
-        <f>F7/F$11</f>
+        <f t="shared" si="4"/>
         <v>7.8299345902270098E-2</v>
       </c>
       <c r="G17" s="6">
-        <f>G7/G$11</f>
+        <f t="shared" si="4"/>
         <v>9.5905651980418338E-2</v>
       </c>
       <c r="H17" s="6">
-        <f>H7/H$11</f>
+        <f t="shared" si="4"/>
         <v>7.6089936934466681E-2</v>
       </c>
       <c r="I17" s="6">
-        <f>I7/I$11</f>
+        <f t="shared" si="4"/>
         <v>0.10173010380622838</v>
       </c>
       <c r="J17" s="6">
-        <f>J7/J$11</f>
+        <f t="shared" si="4"/>
         <v>9.6643247462919593E-2</v>
       </c>
       <c r="K17" s="6">
-        <f>K7/K$11</f>
+        <f t="shared" si="4"/>
         <v>0.10474205315268369</v>
       </c>
       <c r="L17" s="2">
-        <f>L7/L$11</f>
+        <f t="shared" si="4"/>
         <v>9.139346831316994E-2</v>
       </c>
     </row>
@@ -4508,47 +4508,47 @@
         <v>4</v>
       </c>
       <c r="B18" s="6">
-        <f>B8/B$11</f>
+        <f t="shared" ref="B18:L18" si="5">B8/B$11</f>
         <v>0.18607677293428757</v>
       </c>
       <c r="C18" s="6">
-        <f>C8/C$11</f>
+        <f t="shared" si="5"/>
         <v>0.24090731325772388</v>
       </c>
       <c r="D18" s="6">
-        <f>D8/D$11</f>
+        <f t="shared" si="5"/>
         <v>0.20125130344108447</v>
       </c>
       <c r="E18" s="6">
-        <f>E8/E$11</f>
+        <f t="shared" si="5"/>
         <v>0.22517321016166281</v>
       </c>
       <c r="F18" s="6">
-        <f>F8/F$11</f>
+        <f t="shared" si="5"/>
         <v>0.17487495190457869</v>
       </c>
       <c r="G18" s="6">
-        <f>G8/G$11</f>
+        <f t="shared" si="5"/>
         <v>0.21450823319982198</v>
       </c>
       <c r="H18" s="6">
-        <f>H8/H$11</f>
+        <f t="shared" si="5"/>
         <v>0.12969564025226213</v>
       </c>
       <c r="I18" s="6">
-        <f>I8/I$11</f>
+        <f t="shared" si="5"/>
         <v>0.20173010380622838</v>
       </c>
       <c r="J18" s="6">
-        <f>J8/J$11</f>
+        <f t="shared" si="5"/>
         <v>0.20562060889929742</v>
       </c>
       <c r="K18" s="6">
-        <f>K8/K$11</f>
+        <f t="shared" si="5"/>
         <v>0.18377627236407851</v>
       </c>
       <c r="L18" s="2">
-        <f>L8/L$11</f>
+        <f t="shared" si="5"/>
         <v>0.19014187509141436</v>
       </c>
     </row>
@@ -4557,47 +4557,47 @@
         <v>5</v>
       </c>
       <c r="B19" s="6">
-        <f>B9/B$11</f>
+        <f t="shared" ref="B19:L19" si="6">B9/B$11</f>
         <v>0.15029277813923228</v>
       </c>
       <c r="C19" s="6">
-        <f>C9/C$11</f>
+        <f t="shared" si="6"/>
         <v>0.21666014861165428</v>
       </c>
       <c r="D19" s="6">
-        <f>D9/D$11</f>
+        <f t="shared" si="6"/>
         <v>0.14259645464025025</v>
       </c>
       <c r="E19" s="6">
-        <f>E9/E$11</f>
+        <f t="shared" si="6"/>
         <v>0.15588914549653579</v>
       </c>
       <c r="F19" s="6">
-        <f>F9/F$11</f>
+        <f t="shared" si="6"/>
         <v>0.10619469026548672</v>
       </c>
       <c r="G19" s="6">
-        <f>G9/G$11</f>
+        <f t="shared" si="6"/>
         <v>0.13773920783266577</v>
       </c>
       <c r="H19" s="6">
-        <f>H9/H$11</f>
+        <f t="shared" si="6"/>
         <v>8.692075678639978E-2</v>
       </c>
       <c r="I19" s="6">
-        <f>I9/I$11</f>
+        <f t="shared" si="6"/>
         <v>0.11557093425605536</v>
       </c>
       <c r="J19" s="6">
-        <f>J9/J$11</f>
+        <f t="shared" si="6"/>
         <v>9.5862607338017172E-2</v>
       </c>
       <c r="K19" s="6">
-        <f>K9/K$11</f>
+        <f t="shared" si="6"/>
         <v>0.10891089108910891</v>
       </c>
       <c r="L19" s="2">
-        <f>L9/L$11</f>
+        <f t="shared" si="6"/>
         <v>0.12154453707766565</v>
       </c>
     </row>
@@ -4606,47 +4606,47 @@
         <v>6</v>
       </c>
       <c r="B20" s="2">
-        <f>B10/B$11</f>
+        <f t="shared" ref="B20:L20" si="7">B10/B$11</f>
         <v>0.18867924528301888</v>
       </c>
       <c r="C20" s="2">
-        <f>C10/C$11</f>
+        <f t="shared" si="7"/>
         <v>7.1959327336722723E-2</v>
       </c>
       <c r="D20" s="2">
-        <f>D10/D$11</f>
+        <f t="shared" si="7"/>
         <v>0.15276329509906153</v>
       </c>
       <c r="E20" s="2">
-        <f>E10/E$11</f>
+        <f t="shared" si="7"/>
         <v>6.3510392609699776E-2</v>
       </c>
       <c r="F20" s="2">
-        <f>F10/F$11</f>
+        <f t="shared" si="7"/>
         <v>0.14043863024240091</v>
       </c>
       <c r="G20" s="2">
-        <f>G10/G$11</f>
+        <f t="shared" si="7"/>
         <v>6.8535825545171333E-2</v>
       </c>
       <c r="H20" s="2">
-        <f>H10/H$11</f>
+        <f t="shared" si="7"/>
         <v>0.29435152179873869</v>
       </c>
       <c r="I20" s="2">
-        <f>I10/I$11</f>
+        <f t="shared" si="7"/>
         <v>0.23685121107266435</v>
       </c>
       <c r="J20" s="2">
-        <f>J10/J$11</f>
+        <f t="shared" si="7"/>
         <v>0.27447306791569087</v>
       </c>
       <c r="K20" s="2">
-        <f>K10/K$11</f>
+        <f t="shared" si="7"/>
         <v>0.24648254299114122</v>
       </c>
       <c r="L20" s="2">
-        <f>L10/L$11</f>
+        <f t="shared" si="7"/>
         <v>0.19434171211266429</v>
       </c>
     </row>

</xml_diff>

<commit_message>
De cijfers vervangen door namen zoals gevonden in het HW pdf document
</commit_message>
<xml_diff>
--- a/ass_3/Table and Chart of communities per year/Yearly Growth and Shrinkage per community.xlsx
+++ b/ass_3/Table and Chart of communities per year/Yearly Growth and Shrinkage per community.xlsx
@@ -27,24 +27,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Growing and shrinking of communities over the years</t>
-  </si>
-  <si>
-    <t>Community 0</t>
-  </si>
-  <si>
-    <t>Community 1</t>
-  </si>
-  <si>
-    <t>Community 2</t>
-  </si>
-  <si>
-    <t>Community 3</t>
-  </si>
-  <si>
-    <t>Community 4</t>
-  </si>
-  <si>
-    <t>Community 5</t>
   </si>
   <si>
     <t>Total</t>
@@ -84,6 +66,24 @@
   </si>
   <si>
     <t>Number of authors</t>
+  </si>
+  <si>
+    <t>DB (0)</t>
+  </si>
+  <si>
+    <t>AL &amp; ML (1)</t>
+  </si>
+  <si>
+    <t>IR (2)</t>
+  </si>
+  <si>
+    <t>DM (3)</t>
+  </si>
+  <si>
+    <t>AL &amp; TH (4)</t>
+  </si>
+  <si>
+    <t>CV (5)</t>
   </si>
 </sst>
 </file>
@@ -170,6 +170,24 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -367,24 +385,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -756,7 +756,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 0</c:v>
+                  <c:v>DB (0)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -861,7 +861,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 1</c:v>
+                  <c:v>AL &amp; ML (1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -966,7 +966,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 2</c:v>
+                  <c:v>IR (2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1071,7 +1071,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 3</c:v>
+                  <c:v>DM (3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1176,7 +1176,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 4</c:v>
+                  <c:v>AL &amp; TH (4)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1281,7 +1281,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 5</c:v>
+                  <c:v>CV (5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1658,7 +1658,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 0</c:v>
+                  <c:v>DB (0)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1763,7 +1763,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 1</c:v>
+                  <c:v>AL &amp; ML (1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1868,7 +1868,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 2</c:v>
+                  <c:v>IR (2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1973,7 +1973,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 3</c:v>
+                  <c:v>DM (3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2078,7 +2078,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 4</c:v>
+                  <c:v>AL &amp; TH (4)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2183,7 +2183,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Community 5</c:v>
+                  <c:v>CV (5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3677,38 +3677,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A14:L20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A14:L20"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Relative share of attention" dataDxfId="11"/>
-    <tableColumn id="2" name="2001" dataDxfId="10">
+    <tableColumn id="1" name="Relative share of attention" dataDxfId="0"/>
+    <tableColumn id="2" name="2001" dataDxfId="11">
       <calculatedColumnFormula>B5/B$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="2002" dataDxfId="9">
+    <tableColumn id="3" name="2002" dataDxfId="10">
       <calculatedColumnFormula>C5/C$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="2003" dataDxfId="8">
+    <tableColumn id="4" name="2003" dataDxfId="9">
       <calculatedColumnFormula>D5/D$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="2004" dataDxfId="7">
+    <tableColumn id="5" name="2004" dataDxfId="8">
       <calculatedColumnFormula>E5/E$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="2005" dataDxfId="6">
+    <tableColumn id="6" name="2005" dataDxfId="7">
       <calculatedColumnFormula>F5/F$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="2006" dataDxfId="5">
+    <tableColumn id="7" name="2006" dataDxfId="6">
       <calculatedColumnFormula>G5/G$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="2007" dataDxfId="4">
+    <tableColumn id="8" name="2007" dataDxfId="5">
       <calculatedColumnFormula>H5/H$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="2008" dataDxfId="3">
+    <tableColumn id="9" name="2008" dataDxfId="4">
       <calculatedColumnFormula>I5/I$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="2009" dataDxfId="2">
+    <tableColumn id="10" name="2009" dataDxfId="3">
       <calculatedColumnFormula>J5/J$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="2010" dataDxfId="1">
+    <tableColumn id="11" name="2010" dataDxfId="2">
       <calculatedColumnFormula>K5/K$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Total" dataDxfId="0">
+    <tableColumn id="12" name="Total" dataDxfId="1">
       <calculatedColumnFormula>L5/L$11</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3982,7 +3982,7 @@
   <dimension ref="A2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3999,45 +3999,45 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>553</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <v>715</v>
@@ -4115,7 +4115,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>192</v>
@@ -4154,7 +4154,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3">
         <v>572</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3">
         <v>462</v>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3">
         <v>580</v>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" ref="B11:L11" si="1">SUM(B5:B10)</f>
@@ -4320,45 +4320,45 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L14" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6">
         <f t="shared" ref="B15:L15" si="2">B5/B$11</f>
@@ -4407,7 +4407,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6">
         <f t="shared" ref="B16:L16" si="3">B6/B$11</f>
@@ -4456,7 +4456,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6">
         <f t="shared" ref="B17:L17" si="4">B7/B$11</f>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B18" s="6">
         <f t="shared" ref="B18:L18" si="5">B8/B$11</f>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B19" s="6">
         <f t="shared" ref="B19:L19" si="6">B9/B$11</f>
@@ -4603,7 +4603,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20:L20" si="7">B10/B$11</f>

</xml_diff>